<commit_message>
Open existing excel file and write to one cell
</commit_message>
<xml_diff>
--- a/exel_automation/my_workbook.xlsx
+++ b/exel_automation/my_workbook.xlsx
@@ -420,7 +420,15 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Andrew was here</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add file to work with cell contents
</commit_message>
<xml_diff>
--- a/exel_automation/my_workbook.xlsx
+++ b/exel_automation/my_workbook.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,6 +428,13 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ereh saw werdnA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Done manipulating content in excel cells
</commit_message>
<xml_diff>
--- a/exel_automation/my_workbook.xlsx
+++ b/exel_automation/my_workbook.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,6 +434,11 @@
           <t>ereh saw werdnA</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Under reversed</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>